<commit_message>
Feature - Updating the junior developer requirements spreadsheet
</commit_message>
<xml_diff>
--- a/Data/Developer - Junior/Requirements.xlsx
+++ b/Data/Developer - Junior/Requirements.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DominicMartin\GitHub\development-career-roadmap\Data\Developer - Junior\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CE0CC-70E0-4AB5-AB54-04FD754B5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="23620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Must Know</t>
+  </si>
+  <si>
+    <t>Good To Know</t>
+  </si>
+  <si>
+    <t>Bonus Knowledge</t>
+  </si>
+  <si>
+    <t>General Development Skills</t>
+  </si>
+  <si>
+    <t>GIT / Version Control</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>Basic Web Understanding</t>
+  </si>
+  <si>
+    <t>How to search the web</t>
+  </si>
+  <si>
+    <t>.NET</t>
+  </si>
+  <si>
+    <t>Basic C# 11 Syntax</t>
+  </si>
+  <si>
+    <t>Basic .NET CLI commands</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +75,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -45,14 +126,220 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +617,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D5:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="29.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="13" max="13" width="22.90625" customWidth="1"/>
+    <col min="14" max="14" width="20.453125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="M6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
+    </row>
+    <row r="7" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="M7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="10"/>
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="M8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="13"/>
+    </row>
+    <row r="9" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="M9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="M15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="M16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature - Adding XMind file for Junior Dev
</commit_message>
<xml_diff>
--- a/Data/Developer - Junior/Requirements.xlsx
+++ b/Data/Developer - Junior/Requirements.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DominicMartin\GitHub\development-career-roadmap\Data\Developer - Junior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90CE0CC-70E0-4AB5-AB54-04FD754B5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A67F51-82DF-4E18-815F-69092F54F026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="23620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,20 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Key</t>
   </si>
   <si>
-    <t>Must Know</t>
-  </si>
-  <si>
-    <t>Good To Know</t>
-  </si>
-  <si>
-    <t>Bonus Knowledge</t>
-  </si>
-  <si>
     <t>General Development Skills</t>
   </si>
   <si>
@@ -54,13 +46,247 @@
     <t>How to search the web</t>
   </si>
   <si>
-    <t>.NET</t>
-  </si>
-  <si>
-    <t>Basic C# 11 Syntax</t>
-  </si>
-  <si>
-    <t>Basic .NET CLI commands</t>
+    <t>Good to know but not mandatory</t>
+  </si>
+  <si>
+    <t>Bonus knowledge</t>
+  </si>
+  <si>
+    <t>Must know</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
+  </si>
+  <si>
+    <t>Web API</t>
+  </si>
+  <si>
+    <t>C# &amp; .NET Basics</t>
+  </si>
+  <si>
+    <t>C# 11 Syntax</t>
+  </si>
+  <si>
+    <t>.NET CLI commands</t>
+  </si>
+  <si>
+    <t>Middleware</t>
+  </si>
+  <si>
+    <t>Routing</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Basic Database Design</t>
+  </si>
+  <si>
+    <t>Basic SQL Syntax</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Stored Procedures</t>
+  </si>
+  <si>
+    <t>Triggers</t>
+  </si>
+  <si>
+    <t>SOLID Principles</t>
+  </si>
+  <si>
+    <t>Single Responsibility</t>
+  </si>
+  <si>
+    <t>Open-Closed</t>
+  </si>
+  <si>
+    <t>Liskov Substitution</t>
+  </si>
+  <si>
+    <t>Interface Segregation</t>
+  </si>
+  <si>
+    <t>Dependency Inversion</t>
+  </si>
+  <si>
+    <t>Databases - SQL Server</t>
+  </si>
+  <si>
+    <t>Databases - Postgres</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>REST API Basics</t>
+  </si>
+  <si>
+    <t>HTTP Methods</t>
+  </si>
+  <si>
+    <t>CRUD Operations</t>
+  </si>
+  <si>
+    <t>GraphQL</t>
+  </si>
+  <si>
+    <t>gRPC</t>
+  </si>
+  <si>
+    <t>Minimal APIs</t>
+  </si>
+  <si>
+    <t>ORM</t>
+  </si>
+  <si>
+    <t>Entity Framework Basic Operations</t>
+  </si>
+  <si>
+    <t>Code First / Migrations</t>
+  </si>
+  <si>
+    <t>Lazy Loading / Eager Loading</t>
+  </si>
+  <si>
+    <t>Dapper</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Frameworks</t>
+  </si>
+  <si>
+    <t>Mocking</t>
+  </si>
+  <si>
+    <t>Assertions</t>
+  </si>
+  <si>
+    <t>Integration Testing</t>
+  </si>
+  <si>
+    <t>E2E Testing</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Containerisation</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>Orchistratrion</t>
+  </si>
+  <si>
+    <t>Kubernetes</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>What it is</t>
+  </si>
+  <si>
+    <t>Benefite/why it is used</t>
+  </si>
+  <si>
+    <t>Azure Pipelines</t>
+  </si>
+  <si>
+    <t>GitHub Actions</t>
+  </si>
+  <si>
+    <t>TeamCity</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Infrastructure as code</t>
+  </si>
+  <si>
+    <t>Monitoring tools</t>
+  </si>
+  <si>
+    <t>AGILE</t>
+  </si>
+  <si>
+    <t>Overview of the methodologie &amp; manifesto</t>
+  </si>
+  <si>
+    <t>Brief overview of practises</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
+  </si>
+  <si>
+    <t>Microservices</t>
+  </si>
+  <si>
+    <t>Message Broker</t>
+  </si>
+  <si>
+    <t>Why we implement them</t>
+  </si>
+  <si>
+    <t>Problem that they solve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creational </t>
+  </si>
+  <si>
+    <t>Structural</t>
+  </si>
+  <si>
+    <t>Behavioural</t>
+  </si>
+  <si>
+    <t>Soft Skills</t>
+  </si>
+  <si>
+    <t>Good communication</t>
+  </si>
+  <si>
+    <t>Team player</t>
+  </si>
+  <si>
+    <t>Adaptable</t>
+  </si>
+  <si>
+    <t>Eager to learn</t>
+  </si>
+  <si>
+    <t>Empathy</t>
+  </si>
+  <si>
+    <t>Critical Thinker</t>
+  </si>
+  <si>
+    <t>Miscellanous</t>
+  </si>
+  <si>
+    <t>Available Portfolio</t>
+  </si>
+  <si>
+    <t>Shows ability for continue learning</t>
+  </si>
+  <si>
+    <t>Keeps up to date with latest info</t>
+  </si>
+  <si>
+    <t>GG</t>
   </si>
 </sst>
 </file>
@@ -90,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +343,13 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -273,20 +504,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -295,49 +617,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Accent6" xfId="4" builtinId="49"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,103 +902,642 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D5:O16"/>
+  <dimension ref="D5:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="29.81640625" customWidth="1"/>
+    <col min="4" max="4" width="42.81640625" customWidth="1"/>
     <col min="5" max="5" width="12.453125" customWidth="1"/>
     <col min="13" max="13" width="22.90625" customWidth="1"/>
     <col min="14" max="14" width="20.453125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="19" max="19" width="26.7265625" customWidth="1"/>
+    <col min="20" max="20" width="17.81640625" customWidth="1"/>
+    <col min="21" max="21" width="11.90625" customWidth="1"/>
+    <col min="25" max="25" width="28.90625" customWidth="1"/>
+    <col min="26" max="26" width="21" customWidth="1"/>
+    <col min="27" max="27" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D6" s="3" t="s">
+    <row r="5" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D6" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="M6" s="17" t="s">
+      <c r="E6" s="29"/>
+      <c r="M6" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="O6" s="24"/>
+      <c r="S6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="T6" s="23"/>
+      <c r="U6" s="24"/>
+      <c r="Y6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="24"/>
+    </row>
+    <row r="7" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="M7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="17"/>
+      <c r="O7" s="5"/>
+      <c r="S7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="T7" s="17"/>
+      <c r="U7" s="9"/>
+      <c r="Y7" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="5"/>
+    </row>
+    <row r="8" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="M8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="19"/>
+      <c r="O8" s="6"/>
+      <c r="S8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="T8" s="19"/>
+      <c r="U8" s="8"/>
+      <c r="Y8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="M9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="M7" s="9" t="s">
+      <c r="N9" s="19"/>
+      <c r="O9" s="6"/>
+      <c r="S9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="19"/>
+      <c r="U9" s="10"/>
+      <c r="Y9" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="8"/>
+    </row>
+    <row r="10" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
-    </row>
-    <row r="8" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="M8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="13"/>
-    </row>
-    <row r="9" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="M9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="13"/>
-    </row>
-    <row r="10" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="M10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="16"/>
-    </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="M14" s="1" t="s">
+      <c r="N10" s="21"/>
+      <c r="O10" s="7"/>
+      <c r="S10" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="T10" s="21"/>
+      <c r="U10" s="11"/>
+      <c r="Y10" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="8"/>
+    </row>
+    <row r="11" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z11" s="21"/>
+      <c r="AA11" s="12"/>
+    </row>
+    <row r="13" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="23"/>
+      <c r="O14" s="24"/>
+      <c r="S14" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="T14" s="23"/>
+      <c r="U14" s="24"/>
+    </row>
+    <row r="15" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="17"/>
+      <c r="O15" s="5"/>
+      <c r="S15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15" s="17"/>
+      <c r="U15" s="5"/>
+      <c r="Y15" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="24"/>
+    </row>
+    <row r="16" spans="4:27" x14ac:dyDescent="0.35">
+      <c r="M16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="8"/>
+      <c r="S16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="19"/>
+      <c r="U16" s="8"/>
+      <c r="Y16" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="5"/>
+    </row>
+    <row r="17" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="M15" s="1" t="s">
+      <c r="N17" s="19"/>
+      <c r="O17" s="8"/>
+      <c r="S17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="T17" s="19"/>
+      <c r="U17" s="8"/>
+      <c r="Y17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="M16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="1"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="8"/>
+      <c r="S18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T18" s="19"/>
+      <c r="U18" s="8"/>
+      <c r="Y18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M19" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N19" s="19"/>
+      <c r="O19" s="10"/>
+      <c r="S19" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" s="19"/>
+      <c r="U19" s="10"/>
+      <c r="Y19" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N20" s="19"/>
+      <c r="O20" s="10"/>
+      <c r="S20" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="T20" s="21"/>
+      <c r="U20" s="11"/>
+      <c r="Y20" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="10"/>
+      <c r="Y21" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="7"/>
+    </row>
+    <row r="22" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M22" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="21"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S24" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="T24" s="23"/>
+      <c r="U24" s="24"/>
+      <c r="Y24" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="15"/>
+    </row>
+    <row r="25" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S25" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="T25" s="17"/>
+      <c r="U25" s="5"/>
+      <c r="Y25" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="9"/>
+    </row>
+    <row r="26" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M26" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="23"/>
+      <c r="O26" s="24"/>
+      <c r="S26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="T26" s="19"/>
+      <c r="U26" s="6"/>
+      <c r="Y26" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="8"/>
+    </row>
+    <row r="27" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="17"/>
+      <c r="O27" s="5"/>
+      <c r="S27" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="T27" s="19"/>
+      <c r="U27" s="8"/>
+      <c r="Y27" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="12"/>
+    </row>
+    <row r="28" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M28" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N28" s="19"/>
+      <c r="O28" s="6"/>
+      <c r="S28" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="T28" s="19"/>
+      <c r="U28" s="10"/>
+    </row>
+    <row r="29" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M29" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="19"/>
+      <c r="O29" s="8"/>
+      <c r="S29" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="T29" s="21"/>
+      <c r="U29" s="11"/>
+    </row>
+    <row r="30" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M30" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="19"/>
+      <c r="O30" s="8"/>
+    </row>
+    <row r="31" spans="13:27" x14ac:dyDescent="0.35">
+      <c r="M31" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N31" s="19"/>
+      <c r="O31" s="8"/>
+    </row>
+    <row r="32" spans="13:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M32" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" s="19"/>
+      <c r="O32" s="10"/>
+    </row>
+    <row r="33" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M33" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="N33" s="21"/>
+      <c r="O33" s="11"/>
+      <c r="S33" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="T33" s="23"/>
+      <c r="U33" s="24"/>
+    </row>
+    <row r="34" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S34" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="T34" s="17"/>
+      <c r="U34" s="5"/>
+    </row>
+    <row r="35" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J35" t="s">
+        <v>86</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N35" s="23"/>
+      <c r="O35" s="24"/>
+      <c r="S35" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="T35" s="19"/>
+      <c r="U35" s="6"/>
+    </row>
+    <row r="36" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="M36" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="17"/>
+      <c r="O36" s="5"/>
+      <c r="S36" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T36" s="19"/>
+      <c r="U36" s="8"/>
+    </row>
+    <row r="37" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="M37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="N37" s="19"/>
+      <c r="O37" s="6"/>
+      <c r="S37" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="T37" s="19"/>
+      <c r="U37" s="10"/>
+    </row>
+    <row r="38" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M38" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N38" s="19"/>
+      <c r="O38" s="6"/>
+      <c r="S38" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="T38" s="21"/>
+      <c r="U38" s="11"/>
+    </row>
+    <row r="39" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="M39" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N39" s="19"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M40" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" s="21"/>
+      <c r="O40" s="7"/>
+    </row>
+    <row r="41" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S41" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="T41" s="23"/>
+      <c r="U41" s="24"/>
+    </row>
+    <row r="42" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="S42" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="T42" s="17"/>
+      <c r="U42" s="5"/>
+    </row>
+    <row r="43" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="S43" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="T43" s="19"/>
+      <c r="U43" s="10"/>
+    </row>
+    <row r="44" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S44" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T44" s="21"/>
+      <c r="U44" s="11"/>
+    </row>
+    <row r="45" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M45" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N45" s="23"/>
+      <c r="O45" s="24"/>
+    </row>
+    <row r="46" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="M46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" s="17"/>
+      <c r="O46" s="5"/>
+    </row>
+    <row r="47" spans="10:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M47" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47" s="19"/>
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="10:21" x14ac:dyDescent="0.35">
+      <c r="M48" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N48" s="19"/>
+      <c r="O48" s="6"/>
+      <c r="S48" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="T48" s="26"/>
+      <c r="U48" s="27"/>
+    </row>
+    <row r="49" spans="13:21" x14ac:dyDescent="0.35">
+      <c r="M49" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N49" s="19"/>
+      <c r="O49" s="10"/>
+      <c r="S49" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="T49" s="19"/>
+      <c r="U49" s="6"/>
+    </row>
+    <row r="50" spans="13:21" x14ac:dyDescent="0.35">
+      <c r="M50" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N50" s="19"/>
+      <c r="O50" s="10"/>
+      <c r="S50" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="T50" s="19"/>
+      <c r="U50" s="8"/>
+    </row>
+    <row r="51" spans="13:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M51" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="N51" s="21"/>
+      <c r="O51" s="11"/>
+      <c r="S51" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="T51" s="21"/>
+      <c r="U51" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
+  <mergeCells count="85">
+    <mergeCell ref="M10:N10"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S51:T51"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="S42:T42"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="S48:U48"/>
+    <mergeCell ref="S49:T49"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S41:U41"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S27:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>